<commit_message>
Reivisi #1 Data Mahasiswa(no_wa,email,angkatan) jadi satu database
</commit_message>
<xml_diff>
--- a/downloads/data_excel.xlsx
+++ b/downloads/data_excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\si-ci-labkom\uploads\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\si-ci-labkom\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C4D3C6-66FD-449E-9881-E9C0333DE0A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF13474-564F-412C-AFEA-F1CA72FD496C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nim (Ini Buat Input Nim)</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Prodi(Input Prodi)</t>
+  </si>
+  <si>
+    <t>Nomor WA</t>
+  </si>
+  <si>
+    <t>E-Mail</t>
   </si>
 </sst>
 </file>
@@ -401,20 +407,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E17"/>
+  <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="4" width="28" style="1" customWidth="1"/>
+    <col min="5" max="7" width="28.28515625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -427,102 +434,140 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>